<commit_message>
Deploying to gh-pages from @ NIH-NCPI/ncpi-fhir-ig@b7a44ebbae07653767f73d4c5f1972e5a5e69be2 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-disease.xlsx
+++ b/StructureDefinition-disease.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-05-27T12:41:17+00:00</t>
+    <t>2022-08-10T15:01:35+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1395,44 +1395,44 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="35.88671875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="12.65625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="12.66015625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="39.9140625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="6.7734375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="6.77734375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.9453125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="5.4296875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="16.2734375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="13.2578125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="14.44140625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="16.27734375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="13.26171875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="14.4453125" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="72.234375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="72.23828125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="15.265625" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="15.26953125" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="17.16796875" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="17.171875" customWidth="true" bestFit="true"/>
     <col min="21" max="21" width="17.65625" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="19.03125" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="18.85546875" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="85.234375" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="19.03515625" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="18.859375" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="85.23828125" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="56.81640625" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="6.34765625" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="22.71484375" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="20.58984375" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="17.2109375" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="22.71875" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="20.59375" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="17.21484375" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="14.4140625" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="34.859375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="10.55078125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="11.03515625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="13.87109375" customWidth="true" bestFit="true"/>
+    <col min="32" max="32" width="10.5546875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="11.0390625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="13.875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
     <col min="36" max="36" width="29.69921875" customWidth="true" bestFit="true"/>
     <col min="37" max="37" width="255.0" customWidth="true" bestFit="true"/>
     <col min="38" max="38" width="68.20703125" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="222.09765625" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="222.1015625" customWidth="true" bestFit="true"/>
     <col min="40" max="40" width="36.91796875" customWidth="true" bestFit="true"/>
     <col min="41" max="41" width="42.34375" customWidth="true" bestFit="true"/>
   </cols>

</xml_diff>